<commit_message>
ate ao senator bill cassidy
</commit_message>
<xml_diff>
--- a/Twitters_19thCongressMembers.xlsx
+++ b/Twitters_19thCongressMembers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive\Ambiente de Trabalho\tese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDB4397-1F37-4073-86B5-921DCFE763A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D34347D-CD49-4CAE-9B1C-78CF72425115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F8C0650F-6D5B-4461-AA3F-5F73C03E0D01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3936" uniqueCount="1267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3937" uniqueCount="1268">
   <si>
     <t>Name</t>
   </si>
@@ -3837,6 +3837,9 @@
   </si>
   <si>
     <t>"@RepRyanZinke"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -4284,10 +4287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5712D87A-21AD-4759-B6E5-0245C6DE7A64}">
-  <dimension ref="A1:H546"/>
+  <dimension ref="A1:M546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5468,7 +5471,7 @@
       <c r="G45" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="H45" s="12" t="s">
         <v>157</v>
       </c>
     </row>
@@ -5494,7 +5497,7 @@
       <c r="G46" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H46" s="11" t="s">
+      <c r="H46" s="12" t="s">
         <v>160</v>
       </c>
     </row>
@@ -5520,7 +5523,7 @@
       <c r="G47" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H47" s="12" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5546,11 +5549,11 @@
       <c r="G48" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H48" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>166</v>
       </c>
@@ -5572,11 +5575,11 @@
       <c r="G49" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="H49" s="12" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>168</v>
       </c>
@@ -5598,11 +5601,11 @@
       <c r="G50" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H50" s="11" t="s">
+      <c r="H50" s="12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>171</v>
       </c>
@@ -5624,11 +5627,11 @@
       <c r="G51" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="H51" s="12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>173</v>
       </c>
@@ -5650,11 +5653,11 @@
       <c r="G52" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H52" s="12" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>175</v>
       </c>
@@ -5676,11 +5679,11 @@
       <c r="G53" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="H53" s="12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>177</v>
       </c>
@@ -5702,11 +5705,11 @@
       <c r="G54" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="H54" s="12" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>180</v>
       </c>
@@ -5728,11 +5731,11 @@
       <c r="G55" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H55" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>182</v>
       </c>
@@ -5754,11 +5757,11 @@
       <c r="G56" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H56" s="5" t="s">
+      <c r="H56" s="12" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>184</v>
       </c>
@@ -5780,11 +5783,11 @@
       <c r="G57" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="H57" s="12" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>186</v>
       </c>
@@ -5806,11 +5809,11 @@
       <c r="G58" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H58" s="5" t="s">
+      <c r="H58" s="12" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>188</v>
       </c>
@@ -5832,11 +5835,11 @@
       <c r="G59" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="H59" s="12" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>190</v>
       </c>
@@ -5858,11 +5861,11 @@
       <c r="G60" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H60" s="5" t="s">
+      <c r="H60" s="12" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>192</v>
       </c>
@@ -5884,11 +5887,14 @@
       <c r="G61" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H61" s="12" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="M61" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>195</v>
       </c>
@@ -5910,11 +5916,11 @@
       <c r="G62" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="H62" s="12" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>199</v>
       </c>
@@ -5936,11 +5942,11 @@
       <c r="G63" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H63" s="12" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>201</v>
       </c>
@@ -5962,7 +5968,7 @@
       <c r="G64" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H64" s="12" t="s">
         <v>202</v>
       </c>
     </row>
@@ -5988,7 +5994,7 @@
       <c r="G65" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H65" s="12" t="s">
         <v>205</v>
       </c>
     </row>
@@ -6014,7 +6020,7 @@
       <c r="G66" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H66" s="12" t="s">
         <v>207</v>
       </c>
     </row>
@@ -6040,7 +6046,7 @@
       <c r="G67" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H67" s="12" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6066,7 +6072,7 @@
       <c r="G68" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H68" s="12" t="s">
         <v>213</v>
       </c>
     </row>
@@ -6092,7 +6098,7 @@
       <c r="G69" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="H69" s="12" t="s">
         <v>215</v>
       </c>
     </row>
@@ -6118,7 +6124,7 @@
       <c r="G70" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="H70" s="12" t="s">
         <v>219</v>
       </c>
     </row>
@@ -6144,7 +6150,7 @@
       <c r="G71" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H71" s="12" t="s">
         <v>222</v>
       </c>
     </row>
@@ -6170,7 +6176,7 @@
       <c r="G72" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="H72" s="11" t="s">
         <v>224</v>
       </c>
     </row>
@@ -6196,7 +6202,7 @@
       <c r="G73" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="H73" s="11" t="s">
         <v>226</v>
       </c>
     </row>
@@ -6222,7 +6228,7 @@
       <c r="G74" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="H74" s="11" t="s">
         <v>228</v>
       </c>
     </row>
@@ -6248,7 +6254,7 @@
       <c r="G75" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H75" s="5" t="s">
+      <c r="H75" s="11" t="s">
         <v>231</v>
       </c>
     </row>
@@ -6274,7 +6280,7 @@
       <c r="G76" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H76" s="5" t="s">
+      <c r="H76" s="11" t="s">
         <v>234</v>
       </c>
     </row>
@@ -6300,7 +6306,7 @@
       <c r="G77" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H77" s="5" t="s">
+      <c r="H77" s="11" t="s">
         <v>236</v>
       </c>
     </row>
@@ -6326,7 +6332,7 @@
       <c r="G78" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H78" s="5" t="s">
+      <c r="H78" s="11" t="s">
         <v>239</v>
       </c>
     </row>
@@ -6352,7 +6358,7 @@
       <c r="G79" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H79" s="5" t="s">
+      <c r="H79" s="11" t="s">
         <v>241</v>
       </c>
     </row>
@@ -6378,7 +6384,7 @@
       <c r="G80" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H80" s="5" t="s">
+      <c r="H80" s="11" t="s">
         <v>244</v>
       </c>
     </row>

</xml_diff>

<commit_message>
até à judy (tweets por membros)
</commit_message>
<xml_diff>
--- a/Twitters_19thCongressMembers.xlsx
+++ b/Twitters_19thCongressMembers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive\Ambiente de Trabalho\tese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D34347D-CD49-4CAE-9B1C-78CF72425115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A81A4C2-56F8-4A4B-A56A-371FA3AC970F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F8C0650F-6D5B-4461-AA3F-5F73C03E0D01}"/>
   </bookViews>
@@ -4289,8 +4289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5712D87A-21AD-4759-B6E5-0245C6DE7A64}">
   <dimension ref="A1:M546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L63" sqref="L63"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L83" sqref="L83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5972,7 +5972,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>203</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>206</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>208</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>211</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>214</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>216</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>220</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>223</v>
       </c>
@@ -6176,11 +6176,11 @@
       <c r="G72" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H72" s="11" t="s">
+      <c r="H72" s="12" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>225</v>
       </c>
@@ -6202,11 +6202,11 @@
       <c r="G73" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H73" s="11" t="s">
+      <c r="H73" s="12" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>227</v>
       </c>
@@ -6228,11 +6228,11 @@
       <c r="G74" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H74" s="11" t="s">
+      <c r="H74" s="12" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>229</v>
       </c>
@@ -6254,11 +6254,11 @@
       <c r="G75" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H75" s="11" t="s">
+      <c r="H75" s="12" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>232</v>
       </c>
@@ -6280,11 +6280,12 @@
       <c r="G76" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H76" s="11" t="s">
+      <c r="H76" s="12" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>235</v>
       </c>
@@ -6309,8 +6310,9 @@
       <c r="H77" s="11" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>237</v>
       </c>
@@ -6332,11 +6334,11 @@
       <c r="G78" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H78" s="11" t="s">
+      <c r="H78" s="12" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>240</v>
       </c>
@@ -6358,11 +6360,12 @@
       <c r="G79" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H79" s="11" t="s">
+      <c r="H79" s="12" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>242</v>
       </c>
@@ -6384,7 +6387,7 @@
       <c r="G80" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H80" s="11" t="s">
+      <c r="H80" s="12" t="s">
         <v>244</v>
       </c>
     </row>
@@ -6410,7 +6413,7 @@
       <c r="G81" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H81" s="5" t="s">
+      <c r="H81" s="11" t="s">
         <v>247</v>
       </c>
     </row>
@@ -6436,7 +6439,7 @@
       <c r="G82" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H82" s="5" t="s">
+      <c r="H82" s="11" t="s">
         <v>249</v>
       </c>
     </row>
@@ -6462,7 +6465,7 @@
       <c r="G83" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H83" s="5" t="s">
+      <c r="H83" s="11" t="s">
         <v>251</v>
       </c>
     </row>
@@ -6488,7 +6491,7 @@
       <c r="G84" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H84" s="5" t="s">
+      <c r="H84" s="11" t="s">
         <v>253</v>
       </c>
     </row>
@@ -6514,7 +6517,7 @@
       <c r="G85" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H85" s="5" t="s">
+      <c r="H85" s="11" t="s">
         <v>255</v>
       </c>
     </row>
@@ -6540,7 +6543,7 @@
       <c r="G86" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H86" s="5" t="s">
+      <c r="H86" s="11" t="s">
         <v>257</v>
       </c>
     </row>
@@ -6566,7 +6569,7 @@
       <c r="G87" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H87" s="5" t="s">
+      <c r="H87" s="12" t="s">
         <v>259</v>
       </c>
     </row>
@@ -6592,7 +6595,7 @@
       <c r="G88" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H88" s="5" t="s">
+      <c r="H88" s="11" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6618,7 +6621,7 @@
       <c r="G89" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H89" s="5" t="s">
+      <c r="H89" s="12" t="s">
         <v>265</v>
       </c>
     </row>
@@ -6644,7 +6647,7 @@
       <c r="G90" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H90" s="5" t="s">
+      <c r="H90" s="11" t="s">
         <v>268</v>
       </c>
     </row>
@@ -6670,7 +6673,7 @@
       <c r="G91" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H91" s="5" t="s">
+      <c r="H91" s="11" t="s">
         <v>270</v>
       </c>
     </row>
@@ -6696,7 +6699,7 @@
       <c r="G92" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H92" s="5" t="s">
+      <c r="H92" s="11" t="s">
         <v>273</v>
       </c>
     </row>
@@ -6722,7 +6725,7 @@
       <c r="G93" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H93" s="5" t="s">
+      <c r="H93" s="11" t="s">
         <v>276</v>
       </c>
     </row>
@@ -6748,7 +6751,7 @@
       <c r="G94" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H94" s="5" t="s">
+      <c r="H94" s="11" t="s">
         <v>279</v>
       </c>
     </row>
@@ -6774,7 +6777,7 @@
       <c r="G95" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H95" s="5" t="s">
+      <c r="H95" s="11" t="s">
         <v>281</v>
       </c>
     </row>
@@ -6800,7 +6803,7 @@
       <c r="G96" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H96" s="5" t="s">
+      <c r="H96" s="11" t="s">
         <v>284</v>
       </c>
     </row>
@@ -6826,7 +6829,7 @@
       <c r="G97" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H97" s="5" t="s">
+      <c r="H97" s="11" t="s">
         <v>286</v>
       </c>
     </row>
@@ -6852,7 +6855,7 @@
       <c r="G98" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H98" s="5" t="s">
+      <c r="H98" s="11" t="s">
         <v>289</v>
       </c>
     </row>
@@ -6878,7 +6881,7 @@
       <c r="G99" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H99" s="5" t="s">
+      <c r="H99" s="11" t="s">
         <v>291</v>
       </c>
     </row>
@@ -6904,7 +6907,7 @@
       <c r="G100" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H100" s="5" t="s">
+      <c r="H100" s="11" t="s">
         <v>294</v>
       </c>
     </row>
@@ -6930,7 +6933,7 @@
       <c r="G101" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H101" s="5" t="s">
+      <c r="H101" s="11" t="s">
         <v>298</v>
       </c>
     </row>
@@ -6956,7 +6959,7 @@
       <c r="G102" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H102" s="5" t="s">
+      <c r="H102" s="11" t="s">
         <v>300</v>
       </c>
     </row>
@@ -6982,7 +6985,7 @@
       <c r="G103" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H103" s="5" t="s">
+      <c r="H103" s="11" t="s">
         <v>302</v>
       </c>
     </row>
@@ -7008,7 +7011,7 @@
       <c r="G104" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H104" s="5" t="s">
+      <c r="H104" s="11" t="s">
         <v>306</v>
       </c>
     </row>
@@ -7034,7 +7037,7 @@
       <c r="G105" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H105" s="5" t="s">
+      <c r="H105" s="11" t="s">
         <v>308</v>
       </c>
     </row>
@@ -7060,7 +7063,7 @@
       <c r="G106" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H106" s="5" t="s">
+      <c r="H106" s="11" t="s">
         <v>310</v>
       </c>
     </row>
@@ -7086,7 +7089,7 @@
       <c r="G107" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H107" s="5" t="s">
+      <c r="H107" s="11" t="s">
         <v>312</v>
       </c>
     </row>
@@ -7112,7 +7115,7 @@
       <c r="G108" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H108" s="5" t="s">
+      <c r="H108" s="11" t="s">
         <v>314</v>
       </c>
     </row>
@@ -7138,7 +7141,7 @@
       <c r="G109" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H109" s="5" t="s">
+      <c r="H109" s="11" t="s">
         <v>316</v>
       </c>
     </row>
@@ -7164,7 +7167,7 @@
       <c r="G110" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H110" s="5" t="s">
+      <c r="H110" s="11" t="s">
         <v>318</v>
       </c>
     </row>
@@ -7190,7 +7193,7 @@
       <c r="G111" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H111" s="5" t="s">
+      <c r="H111" s="11" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7216,7 +7219,7 @@
       <c r="G112" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H112" s="5" t="s">
+      <c r="H112" s="11" t="s">
         <v>324</v>
       </c>
     </row>
@@ -7242,7 +7245,7 @@
       <c r="G113" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H113" s="5" t="s">
+      <c r="H113" s="11" t="s">
         <v>327</v>
       </c>
     </row>
@@ -7268,7 +7271,7 @@
       <c r="G114" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H114" s="5" t="s">
+      <c r="H114" s="11" t="s">
         <v>329</v>
       </c>
     </row>
@@ -7294,7 +7297,7 @@
       <c r="G115" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H115" s="5" t="s">
+      <c r="H115" s="11" t="s">
         <v>331</v>
       </c>
     </row>
@@ -7320,7 +7323,7 @@
       <c r="G116" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H116" s="5" t="s">
+      <c r="H116" s="11" t="s">
         <v>333</v>
       </c>
     </row>
@@ -7346,7 +7349,7 @@
       <c r="G117" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H117" s="5" t="s">
+      <c r="H117" s="11" t="s">
         <v>335</v>
       </c>
     </row>
@@ -7372,7 +7375,7 @@
       <c r="G118" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H118" s="5" t="s">
+      <c r="H118" s="11" t="s">
         <v>337</v>
       </c>
     </row>
@@ -7398,7 +7401,7 @@
       <c r="G119" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H119" s="5" t="s">
+      <c r="H119" s="11" t="s">
         <v>339</v>
       </c>
     </row>
@@ -7424,7 +7427,7 @@
       <c r="G120" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H120" s="5" t="s">
+      <c r="H120" s="11" t="s">
         <v>342</v>
       </c>
     </row>
@@ -7450,7 +7453,7 @@
       <c r="G121" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H121" s="5" t="s">
+      <c r="H121" s="11" t="s">
         <v>344</v>
       </c>
     </row>
@@ -7476,7 +7479,7 @@
       <c r="G122" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H122" s="5" t="s">
+      <c r="H122" s="11" t="s">
         <v>346</v>
       </c>
     </row>
@@ -7502,7 +7505,7 @@
       <c r="G123" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H123" s="5" t="s">
+      <c r="H123" s="11" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7528,7 +7531,7 @@
       <c r="G124" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H124" s="5" t="s">
+      <c r="H124" s="11" t="s">
         <v>350</v>
       </c>
     </row>
@@ -7554,7 +7557,7 @@
       <c r="G125" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H125" s="5" t="s">
+      <c r="H125" s="11" t="s">
         <v>352</v>
       </c>
     </row>
@@ -7580,7 +7583,7 @@
       <c r="G126" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H126" s="5" t="s">
+      <c r="H126" s="11" t="s">
         <v>354</v>
       </c>
     </row>
@@ -7606,7 +7609,7 @@
       <c r="G127" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H127" s="5" t="s">
+      <c r="H127" s="11" t="s">
         <v>356</v>
       </c>
     </row>
@@ -7632,7 +7635,7 @@
       <c r="G128" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H128" s="5" t="s">
+      <c r="H128" s="11" t="s">
         <v>359</v>
       </c>
     </row>
@@ -7658,7 +7661,7 @@
       <c r="G129" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H129" s="5" t="s">
+      <c r="H129" s="11" t="s">
         <v>361</v>
       </c>
     </row>
@@ -7684,7 +7687,7 @@
       <c r="G130" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H130" s="5" t="s">
+      <c r="H130" s="11" t="s">
         <v>363</v>
       </c>
     </row>
@@ -7710,7 +7713,7 @@
       <c r="G131" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H131" s="5" t="s">
+      <c r="H131" s="11" t="s">
         <v>366</v>
       </c>
     </row>
@@ -7736,7 +7739,7 @@
       <c r="G132" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H132" s="5" t="s">
+      <c r="H132" s="11" t="s">
         <v>368</v>
       </c>
     </row>
@@ -7762,7 +7765,7 @@
       <c r="G133" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H133" s="5" t="s">
+      <c r="H133" s="11" t="s">
         <v>141</v>
       </c>
     </row>
@@ -7788,7 +7791,7 @@
       <c r="G134" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H134" s="5" t="s">
+      <c r="H134" s="11" t="s">
         <v>372</v>
       </c>
     </row>
@@ -7814,7 +7817,7 @@
       <c r="G135" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H135" s="5" t="s">
+      <c r="H135" s="11" t="s">
         <v>374</v>
       </c>
     </row>
@@ -7840,7 +7843,7 @@
       <c r="G136" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H136" s="5" t="s">
+      <c r="H136" s="11" t="s">
         <v>376</v>
       </c>
     </row>
@@ -7866,7 +7869,7 @@
       <c r="G137" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H137" s="5" t="s">
+      <c r="H137" s="11" t="s">
         <v>378</v>
       </c>
     </row>
@@ -7892,7 +7895,7 @@
       <c r="G138" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H138" s="5" t="s">
+      <c r="H138" s="11" t="s">
         <v>382</v>
       </c>
     </row>
@@ -7918,7 +7921,7 @@
       <c r="G139" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H139" s="5" t="s">
+      <c r="H139" s="11" t="s">
         <v>384</v>
       </c>
     </row>
@@ -7944,7 +7947,7 @@
       <c r="G140" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H140" s="5" t="s">
+      <c r="H140" s="11" t="s">
         <v>386</v>
       </c>
     </row>
@@ -7970,7 +7973,7 @@
       <c r="G141" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H141" s="5" t="s">
+      <c r="H141" s="11" t="s">
         <v>388</v>
       </c>
     </row>
@@ -7996,7 +7999,7 @@
       <c r="G142" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H142" s="5" t="s">
+      <c r="H142" s="11" t="s">
         <v>390</v>
       </c>
     </row>
@@ -8022,7 +8025,7 @@
       <c r="G143" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H143" s="5" t="s">
+      <c r="H143" s="11" t="s">
         <v>392</v>
       </c>
     </row>
@@ -8048,7 +8051,7 @@
       <c r="G144" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H144" s="5" t="s">
+      <c r="H144" s="11" t="s">
         <v>395</v>
       </c>
     </row>
@@ -8074,7 +8077,7 @@
       <c r="G145" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H145" s="5" t="s">
+      <c r="H145" s="11" t="s">
         <v>397</v>
       </c>
     </row>
@@ -8100,7 +8103,7 @@
       <c r="G146" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H146" s="5" t="s">
+      <c r="H146" s="11" t="s">
         <v>399</v>
       </c>
     </row>
@@ -8126,7 +8129,7 @@
       <c r="G147" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H147" s="5" t="s">
+      <c r="H147" s="11" t="s">
         <v>401</v>
       </c>
     </row>
@@ -8152,7 +8155,7 @@
       <c r="G148" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H148" s="5" t="s">
+      <c r="H148" s="11" t="s">
         <v>403</v>
       </c>
     </row>
@@ -8178,7 +8181,7 @@
       <c r="G149" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H149" s="5" t="s">
+      <c r="H149" s="11" t="s">
         <v>406</v>
       </c>
     </row>
@@ -8204,7 +8207,7 @@
       <c r="G150" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H150" s="5" t="s">
+      <c r="H150" s="11" t="s">
         <v>408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change date to 25 set 2024
</commit_message>
<xml_diff>
--- a/Twitters_19thCongressMembers.xlsx
+++ b/Twitters_19thCongressMembers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive\Ambiente de Trabalho\tese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A81A4C2-56F8-4A4B-A56A-371FA3AC970F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548ACADF-1919-4F26-85CD-6E278A8FACD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F8C0650F-6D5B-4461-AA3F-5F73C03E0D01}"/>
   </bookViews>
@@ -3873,24 +3873,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDAF2D0"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -3917,7 +3905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3934,9 +3922,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3944,13 +3929,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4289,8 +4274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5712D87A-21AD-4759-B6E5-0245C6DE7A64}">
   <dimension ref="A1:M546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L83" sqref="L83"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4353,7 +4338,7 @@
       <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4379,7 +4364,7 @@
       <c r="G3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4405,7 +4390,7 @@
       <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4431,7 +4416,7 @@
       <c r="G5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4457,7 +4442,7 @@
       <c r="G6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4483,7 +4468,7 @@
       <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4509,7 +4494,7 @@
       <c r="G8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4535,7 +4520,7 @@
       <c r="G9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="11" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4561,7 +4546,7 @@
       <c r="G10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4587,7 +4572,7 @@
       <c r="G11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4613,7 +4598,7 @@
       <c r="G12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="11" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4639,7 +4624,7 @@
       <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="11" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4665,7 +4650,7 @@
       <c r="G14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4691,7 +4676,7 @@
       <c r="G15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="11" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4717,7 +4702,7 @@
       <c r="G16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="11" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4743,7 +4728,7 @@
       <c r="G17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="11" t="s">
         <v>72</v>
       </c>
     </row>
@@ -4769,7 +4754,7 @@
       <c r="G18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4795,7 +4780,7 @@
       <c r="G19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="11" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4821,7 +4806,7 @@
       <c r="G20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="11" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4847,7 +4832,7 @@
       <c r="G21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="11" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4873,7 +4858,7 @@
       <c r="G22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="11" t="s">
         <v>89</v>
       </c>
     </row>
@@ -4899,7 +4884,7 @@
       <c r="G23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="11" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4925,7 +4910,7 @@
       <c r="G24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="11" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4951,7 +4936,7 @@
       <c r="G25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="11" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4977,7 +4962,7 @@
       <c r="G26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="11" t="s">
         <v>100</v>
       </c>
     </row>
@@ -5003,7 +4988,7 @@
       <c r="G27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="11" t="s">
         <v>103</v>
       </c>
     </row>
@@ -5029,7 +5014,7 @@
       <c r="G28" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="11" t="s">
         <v>105</v>
       </c>
     </row>
@@ -5055,7 +5040,7 @@
       <c r="G29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="11" t="s">
         <v>109</v>
       </c>
     </row>
@@ -5081,7 +5066,7 @@
       <c r="G30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="11" t="s">
         <v>112</v>
       </c>
     </row>
@@ -5107,7 +5092,7 @@
       <c r="G31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="11" t="s">
         <v>114</v>
       </c>
     </row>
@@ -5133,7 +5118,7 @@
       <c r="G32" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="11" t="s">
         <v>116</v>
       </c>
     </row>
@@ -5159,7 +5144,7 @@
       <c r="G33" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="11" t="s">
         <v>119</v>
       </c>
     </row>
@@ -5185,7 +5170,7 @@
       <c r="G34" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H34" s="11" t="s">
         <v>122</v>
       </c>
     </row>
@@ -5211,7 +5196,7 @@
       <c r="G35" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="H35" s="11" t="s">
         <v>124</v>
       </c>
     </row>
@@ -5237,7 +5222,7 @@
       <c r="G36" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="11" t="s">
         <v>127</v>
       </c>
     </row>
@@ -5263,7 +5248,7 @@
       <c r="G37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="H37" s="11" t="s">
         <v>130</v>
       </c>
     </row>
@@ -5289,7 +5274,7 @@
       <c r="G38" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="H38" s="11" t="s">
         <v>133</v>
       </c>
     </row>
@@ -5315,7 +5300,7 @@
       <c r="G39" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="10" t="s">
+      <c r="H39" s="11" t="s">
         <v>137</v>
       </c>
     </row>
@@ -5341,7 +5326,7 @@
       <c r="G40" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H40" s="10" t="s">
+      <c r="H40" s="11" t="s">
         <v>141</v>
       </c>
     </row>
@@ -5367,7 +5352,7 @@
       <c r="G41" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="H41" s="11" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5393,7 +5378,7 @@
       <c r="G42" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H42" s="12" t="s">
+      <c r="H42" s="11" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5419,7 +5404,7 @@
       <c r="G43" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H43" s="12" t="s">
+      <c r="H43" s="11" t="s">
         <v>149</v>
       </c>
     </row>
@@ -5445,7 +5430,7 @@
       <c r="G44" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H44" s="12" t="s">
+      <c r="H44" s="11" t="s">
         <v>153</v>
       </c>
     </row>
@@ -5471,7 +5456,7 @@
       <c r="G45" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H45" s="12" t="s">
+      <c r="H45" s="11" t="s">
         <v>157</v>
       </c>
     </row>
@@ -5497,7 +5482,7 @@
       <c r="G46" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H46" s="12" t="s">
+      <c r="H46" s="11" t="s">
         <v>160</v>
       </c>
     </row>
@@ -5523,7 +5508,7 @@
       <c r="G47" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H47" s="12" t="s">
+      <c r="H47" s="11" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5549,7 +5534,7 @@
       <c r="G48" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H48" s="12" t="s">
+      <c r="H48" s="11" t="s">
         <v>165</v>
       </c>
     </row>
@@ -5575,7 +5560,7 @@
       <c r="G49" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="12" t="s">
+      <c r="H49" s="11" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5601,7 +5586,7 @@
       <c r="G50" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H50" s="12" t="s">
+      <c r="H50" s="11" t="s">
         <v>170</v>
       </c>
     </row>
@@ -5627,7 +5612,7 @@
       <c r="G51" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H51" s="12" t="s">
+      <c r="H51" s="11" t="s">
         <v>172</v>
       </c>
     </row>
@@ -5653,7 +5638,7 @@
       <c r="G52" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H52" s="12" t="s">
+      <c r="H52" s="11" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5679,7 +5664,7 @@
       <c r="G53" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H53" s="12" t="s">
+      <c r="H53" s="11" t="s">
         <v>176</v>
       </c>
     </row>
@@ -5705,7 +5690,7 @@
       <c r="G54" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H54" s="12" t="s">
+      <c r="H54" s="11" t="s">
         <v>179</v>
       </c>
     </row>
@@ -5731,7 +5716,7 @@
       <c r="G55" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H55" s="12" t="s">
+      <c r="H55" s="11" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5757,7 +5742,7 @@
       <c r="G56" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H56" s="12" t="s">
+      <c r="H56" s="11" t="s">
         <v>183</v>
       </c>
     </row>
@@ -5783,7 +5768,7 @@
       <c r="G57" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H57" s="12" t="s">
+      <c r="H57" s="11" t="s">
         <v>185</v>
       </c>
     </row>
@@ -5809,7 +5794,7 @@
       <c r="G58" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H58" s="12" t="s">
+      <c r="H58" s="11" t="s">
         <v>187</v>
       </c>
     </row>
@@ -5835,7 +5820,7 @@
       <c r="G59" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H59" s="12" t="s">
+      <c r="H59" s="11" t="s">
         <v>189</v>
       </c>
     </row>
@@ -5861,7 +5846,7 @@
       <c r="G60" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H60" s="12" t="s">
+      <c r="H60" s="11" t="s">
         <v>191</v>
       </c>
     </row>
@@ -5887,7 +5872,7 @@
       <c r="G61" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H61" s="12" t="s">
+      <c r="H61" s="11" t="s">
         <v>194</v>
       </c>
       <c r="M61" t="s">
@@ -5916,7 +5901,7 @@
       <c r="G62" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H62" s="12" t="s">
+      <c r="H62" s="11" t="s">
         <v>198</v>
       </c>
     </row>
@@ -5942,7 +5927,7 @@
       <c r="G63" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H63" s="12" t="s">
+      <c r="H63" s="11" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5968,7 +5953,7 @@
       <c r="G64" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H64" s="12" t="s">
+      <c r="H64" s="11" t="s">
         <v>202</v>
       </c>
     </row>
@@ -5994,7 +5979,7 @@
       <c r="G65" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H65" s="12" t="s">
+      <c r="H65" s="11" t="s">
         <v>205</v>
       </c>
     </row>
@@ -6020,7 +6005,7 @@
       <c r="G66" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H66" s="12" t="s">
+      <c r="H66" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -6046,7 +6031,7 @@
       <c r="G67" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H67" s="12" t="s">
+      <c r="H67" s="11" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6072,7 +6057,7 @@
       <c r="G68" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H68" s="12" t="s">
+      <c r="H68" s="11" t="s">
         <v>213</v>
       </c>
     </row>
@@ -6098,7 +6083,7 @@
       <c r="G69" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H69" s="12" t="s">
+      <c r="H69" s="11" t="s">
         <v>215</v>
       </c>
     </row>
@@ -6124,7 +6109,7 @@
       <c r="G70" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H70" s="12" t="s">
+      <c r="H70" s="11" t="s">
         <v>219</v>
       </c>
     </row>
@@ -6150,7 +6135,7 @@
       <c r="G71" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H71" s="12" t="s">
+      <c r="H71" s="11" t="s">
         <v>222</v>
       </c>
     </row>
@@ -6176,7 +6161,7 @@
       <c r="G72" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H72" s="12" t="s">
+      <c r="H72" s="11" t="s">
         <v>224</v>
       </c>
     </row>
@@ -6202,7 +6187,7 @@
       <c r="G73" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H73" s="12" t="s">
+      <c r="H73" s="11" t="s">
         <v>226</v>
       </c>
     </row>
@@ -6228,7 +6213,7 @@
       <c r="G74" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H74" s="12" t="s">
+      <c r="H74" s="11" t="s">
         <v>228</v>
       </c>
     </row>
@@ -6254,7 +6239,7 @@
       <c r="G75" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H75" s="12" t="s">
+      <c r="H75" s="11" t="s">
         <v>231</v>
       </c>
     </row>
@@ -6280,7 +6265,7 @@
       <c r="G76" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H76" s="12" t="s">
+      <c r="H76" s="11" t="s">
         <v>234</v>
       </c>
       <c r="I76" s="5"/>
@@ -6334,7 +6319,7 @@
       <c r="G78" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H78" s="12" t="s">
+      <c r="H78" s="11" t="s">
         <v>239</v>
       </c>
     </row>
@@ -6360,7 +6345,7 @@
       <c r="G79" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H79" s="12" t="s">
+      <c r="H79" s="11" t="s">
         <v>241</v>
       </c>
       <c r="I79" s="5"/>
@@ -6387,7 +6372,7 @@
       <c r="G80" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H80" s="12" t="s">
+      <c r="H80" s="11" t="s">
         <v>244</v>
       </c>
     </row>
@@ -6569,7 +6554,7 @@
       <c r="G87" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H87" s="12" t="s">
+      <c r="H87" s="11" t="s">
         <v>259</v>
       </c>
     </row>
@@ -6621,7 +6606,7 @@
       <c r="G89" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H89" s="12" t="s">
+      <c r="H89" s="11" t="s">
         <v>265</v>
       </c>
     </row>
@@ -8233,7 +8218,7 @@
       <c r="G151" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H151" s="5" t="s">
+      <c r="H151" s="11" t="s">
         <v>410</v>
       </c>
     </row>
@@ -8259,7 +8244,7 @@
       <c r="G152" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H152" s="5" t="s">
+      <c r="H152" s="11" t="s">
         <v>412</v>
       </c>
     </row>
@@ -8285,7 +8270,7 @@
       <c r="G153" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H153" s="5" t="s">
+      <c r="H153" s="11" t="s">
         <v>412</v>
       </c>
     </row>
@@ -8311,7 +8296,7 @@
       <c r="G154" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H154" s="5" t="s">
+      <c r="H154" s="11" t="s">
         <v>415</v>
       </c>
     </row>
@@ -16345,7 +16330,7 @@
       <c r="G463" s="5" t="s">
         <v>1086</v>
       </c>
-      <c r="H463" s="7"/>
+      <c r="H463" s="6"/>
     </row>
     <row r="464" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A464" s="3" t="s">
@@ -16577,7 +16562,7 @@
       <c r="G472" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H472" s="8" t="s">
+      <c r="H472" s="7" t="s">
         <v>1103</v>
       </c>
     </row>
@@ -17851,7 +17836,7 @@
       <c r="G521" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H521" s="9" t="s">
+      <c r="H521" s="8" t="s">
         <v>1211</v>
       </c>
     </row>

</xml_diff>